<commit_message>
Updates to Questionaire Response
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bfs.xlsx
+++ b/build/output/StructureDefinition-pacio-bfs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="409">
   <si>
     <t>Path</t>
   </si>
@@ -512,10 +512,7 @@
     <t>Used for filtering what observations are retrieved and displayed.</t>
   </si>
   <si>
-    <t>Codes for high level observation categories.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-category</t>
+    <t>http://terminology.hl7.org/CodeSystem/observation-category</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode="COMP].target[classCode="LIST", moodCode="EVN"].code</t>
@@ -1482,7 +1479,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="60.515625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="50.89453125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="56.66015625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
@@ -3159,10 +3156,10 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>45</v>
@@ -3213,11 +3210,9 @@
       <c r="W15" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="X15" t="s" s="2">
+      <c r="X15" s="2"/>
+      <c r="Y15" t="s" s="2">
         <v>158</v>
-      </c>
-      <c r="Y15" t="s" s="2">
-        <v>159</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3259,10 +3254,10 @@
         <v>45</v>
       </c>
       <c r="AM15" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AN15" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="AN15" t="s" s="2">
-        <v>161</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3270,11 +3265,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3296,16 +3291,16 @@
         <v>153</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="M16" t="s" s="2">
+      <c r="N16" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>167</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3334,7 +3329,7 @@
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3352,7 +3347,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>55</v>
@@ -3367,27 +3362,27 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>169</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AL16" t="s" s="2">
         <v>170</v>
       </c>
-      <c r="AL16" t="s" s="2">
+      <c r="AM16" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="AM16" t="s" s="2">
+      <c r="AN16" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="AN16" t="s" s="2">
+      <c r="AO16" t="s" s="2">
         <v>173</v>
-      </c>
-      <c r="AO16" t="s" s="2">
-        <v>174</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3410,19 +3405,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>178</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>179</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>180</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3471,7 +3466,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3486,19 +3481,19 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL17" t="s" s="2">
         <v>181</v>
       </c>
-      <c r="AK17" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL17" t="s" s="2">
+      <c r="AM17" t="s" s="2">
         <v>182</v>
       </c>
-      <c r="AM17" t="s" s="2">
+      <c r="AN17" t="s" s="2">
         <v>183</v>
-      </c>
-      <c r="AN17" t="s" s="2">
-        <v>184</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3506,7 +3501,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3529,16 +3524,16 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>187</v>
       </c>
-      <c r="L18" t="s" s="2">
+      <c r="M18" t="s" s="2">
         <v>188</v>
-      </c>
-      <c r="M18" t="s" s="2">
-        <v>189</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3588,7 +3583,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3609,13 +3604,13 @@
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3623,11 +3618,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3646,19 +3641,19 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>193</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>194</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="M19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>197</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3707,7 +3702,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3722,19 +3717,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="AK19" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL19" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="AK19" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL19" t="s" s="2">
+      <c r="AM19" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="AM19" t="s" s="2">
+      <c r="AN19" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="AN19" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3742,11 +3737,11 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3765,19 +3760,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>206</v>
       </c>
-      <c r="M20" t="s" s="2">
+      <c r="N20" t="s" s="2">
         <v>207</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>208</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3826,7 +3821,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3841,19 +3836,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="AK20" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL20" t="s" s="2">
         <v>209</v>
       </c>
-      <c r="AK20" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL20" t="s" s="2">
+      <c r="AM20" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="AM20" t="s" s="2">
+      <c r="AN20" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="AN20" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3861,7 +3856,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3884,16 +3879,16 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="K21" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="L21" t="s" s="2">
         <v>215</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>216</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>217</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3943,7 +3938,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3964,13 +3959,13 @@
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="AM21" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -3978,7 +3973,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4001,17 +3996,17 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="K22" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="L22" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4060,7 +4055,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4075,19 +4070,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="AK22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL22" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL22" t="s" s="2">
+      <c r="AM22" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AM22" t="s" s="2">
+      <c r="AN22" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4095,7 +4090,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4121,16 +4116,16 @@
         <v>153</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>233</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>234</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4179,7 +4174,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4188,7 +4183,7 @@
         <v>55</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>67</v>
@@ -4197,24 +4192,24 @@
         <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="AL23" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="AL23" t="s" s="2">
+      <c r="AM23" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="AM23" t="s" s="2">
+      <c r="AN23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO23" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO23" t="s" s="2">
-        <v>239</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4240,16 +4235,16 @@
         <v>153</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="M24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>243</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>244</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4274,14 +4269,14 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="X24" t="s" s="2">
         <v>245</v>
       </c>
-      <c r="X24" t="s" s="2">
+      <c r="Y24" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="Y24" t="s" s="2">
-        <v>247</v>
-      </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
       </c>
@@ -4298,7 +4293,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4307,7 +4302,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4322,7 +4317,7 @@
         <v>98</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
@@ -4333,11 +4328,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4359,16 +4354,16 @@
         <v>153</v>
       </c>
       <c r="K25" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L25" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="L25" t="s" s="2">
+      <c r="M25" t="s" s="2">
         <v>253</v>
       </c>
-      <c r="M25" t="s" s="2">
+      <c r="N25" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4393,14 +4388,14 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="X25" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="Y25" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="Y25" t="s" s="2">
-        <v>257</v>
-      </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
       </c>
@@ -4417,7 +4412,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4435,24 +4430,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AL25" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="AL25" t="s" s="2">
+      <c r="AM25" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="AM25" t="s" s="2">
+      <c r="AN25" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO25" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="AN25" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO25" t="s" s="2">
-        <v>261</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4475,19 +4470,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="K26" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="L26" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>265</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>267</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4536,7 +4531,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4557,10 +4552,10 @@
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AM26" t="s" s="2">
         <v>268</v>
-      </c>
-      <c r="AM26" t="s" s="2">
-        <v>269</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4571,7 +4566,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4597,13 +4592,13 @@
         <v>153</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="M27" t="s" s="2">
         <v>272</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4629,14 +4624,14 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="X27" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="X27" t="s" s="2">
+      <c r="Y27" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="Y27" t="s" s="2">
-        <v>276</v>
-      </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4653,7 +4648,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4671,24 +4666,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="AL27" t="s" s="2">
+      <c r="AM27" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="AM27" t="s" s="2">
+      <c r="AN27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO27" t="s" s="2">
         <v>279</v>
-      </c>
-      <c r="AN27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO27" t="s" s="2">
-        <v>280</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4714,16 +4709,16 @@
         <v>153</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="M28" t="s" s="2">
+      <c r="N28" t="s" s="2">
         <v>284</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>285</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4748,14 +4743,14 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="X28" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="Y28" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="Y28" t="s" s="2">
-        <v>287</v>
-      </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4772,7 +4767,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4793,10 +4788,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="AM28" t="s" s="2">
         <v>288</v>
-      </c>
-      <c r="AM28" t="s" s="2">
-        <v>289</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4807,7 +4802,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4830,16 +4825,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>292</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>293</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4889,7 +4884,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4907,24 +4902,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AL29" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AM29" t="s" s="2">
         <v>296</v>
       </c>
-      <c r="AM29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO29" t="s" s="2">
         <v>297</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO29" t="s" s="2">
-        <v>298</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4947,16 +4942,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5006,7 +5001,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5024,24 +5019,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="AL30" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="AL30" t="s" s="2">
+      <c r="AM30" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="AM30" t="s" s="2">
+      <c r="AN30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO30" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>307</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5064,19 +5059,19 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5125,7 +5120,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5137,19 +5132,19 @@
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="AJ31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL31" t="s" s="2">
+      <c r="AM31" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5160,7 +5155,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5186,10 +5181,10 @@
         <v>57</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5240,7 +5235,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5264,7 +5259,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5275,7 +5270,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5304,7 +5299,7 @@
         <v>102</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>104</v>
@@ -5357,7 +5352,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5381,7 +5376,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5392,11 +5387,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5418,10 +5413,10 @@
         <v>101</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>104</v>
@@ -5476,7 +5471,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5511,7 +5506,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5534,13 +5529,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="K35" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="K35" t="s" s="2">
+      <c r="L35" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5591,7 +5586,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5600,7 +5595,7 @@
         <v>55</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>67</v>
@@ -5612,10 +5607,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5626,7 +5621,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5649,13 +5644,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5706,7 +5701,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5715,7 +5710,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5727,10 +5722,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5741,7 +5736,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5767,16 +5762,16 @@
         <v>153</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5804,11 +5799,11 @@
         <v>79</v>
       </c>
       <c r="X37" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="Y37" t="s" s="2">
         <v>346</v>
       </c>
-      <c r="Y37" t="s" s="2">
-        <v>347</v>
-      </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5825,7 +5820,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5843,13 +5838,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="AL37" t="s" s="2">
-        <v>349</v>
-      </c>
       <c r="AM37" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5860,7 +5855,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5886,16 +5881,16 @@
         <v>153</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5920,14 +5915,14 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="X38" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="Y38" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="Y38" t="s" s="2">
-        <v>356</v>
-      </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5944,7 +5939,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5962,13 +5957,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="AL38" t="s" s="2">
-        <v>349</v>
-      </c>
       <c r="AM38" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5979,7 +5974,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6002,17 +5997,17 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>360</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6061,7 +6056,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6085,7 +6080,7 @@
         <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6096,7 +6091,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6122,10 +6117,10 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>364</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6176,7 +6171,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6197,10 +6192,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6211,7 +6206,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6234,16 +6229,16 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="K41" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="L41" t="s" s="2">
         <v>369</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>371</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -6293,7 +6288,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6314,10 +6309,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="AM41" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6328,7 +6323,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6351,16 +6346,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>375</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6410,7 +6405,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6431,10 +6426,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6445,7 +6440,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6468,19 +6463,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>382</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>383</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>384</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6529,7 +6524,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6550,10 +6545,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AM43" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6564,7 +6559,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6590,10 +6585,10 @@
         <v>57</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6644,7 +6639,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6668,7 +6663,7 @@
         <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6679,7 +6674,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6708,7 +6703,7 @@
         <v>102</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
@@ -6761,7 +6756,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6785,7 +6780,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6796,11 +6791,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6822,10 +6817,10 @@
         <v>101</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>104</v>
@@ -6880,7 +6875,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6915,7 +6910,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6941,16 +6936,16 @@
         <v>153</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="M47" t="s" s="2">
-        <v>393</v>
-      </c>
       <c r="N47" t="s" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -6975,14 +6970,14 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="X47" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="Y47" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="Y47" t="s" s="2">
-        <v>395</v>
-      </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
       </c>
@@ -6999,7 +6994,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>55</v>
@@ -7017,16 +7012,16 @@
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AL47" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AM47" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="AM47" t="s" s="2">
+      <c r="AN47" t="s" s="2">
         <v>172</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>173</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7034,7 +7029,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7057,19 +7052,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="K48" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="K48" t="s" s="2">
+      <c r="L48" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="L48" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>400</v>
-      </c>
       <c r="N48" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7118,7 +7113,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7136,24 +7131,24 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AL48" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="AM48" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="AM48" t="s" s="2">
+      <c r="AN48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>239</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7179,16 +7174,16 @@
         <v>153</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="M49" t="s" s="2">
-        <v>405</v>
-      </c>
       <c r="N49" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7213,14 +7208,14 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="X49" t="s" s="2">
         <v>245</v>
       </c>
-      <c r="X49" t="s" s="2">
+      <c r="Y49" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="Y49" t="s" s="2">
-        <v>247</v>
-      </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7237,7 +7232,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7246,7 +7241,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7261,7 +7256,7 @@
         <v>98</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7272,11 +7267,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7298,16 +7293,16 @@
         <v>153</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="M50" t="s" s="2">
         <v>253</v>
       </c>
-      <c r="M50" t="s" s="2">
+      <c r="N50" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7332,14 +7327,14 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="X50" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="Y50" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="Y50" t="s" s="2">
-        <v>257</v>
-      </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
       </c>
@@ -7356,7 +7351,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7374,24 +7369,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AL50" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="AL50" t="s" s="2">
+      <c r="AM50" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="AM50" t="s" s="2">
+      <c r="AN50" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO50" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>261</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7417,16 +7412,16 @@
         <v>45</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="L51" t="s" s="2">
-        <v>409</v>
-      </c>
       <c r="M51" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="N51" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7475,7 +7470,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7496,10 +7491,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="AM51" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
Add build folder with good contents
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bfs.xlsx
+++ b/build/output/StructureDefinition-pacio-bfs.xlsx
@@ -1455,47 +1455,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.6015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="44.67578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="66.26953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="67.91015625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="60.515625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="56.66015625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="63.703125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="57.1328125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="41.01953125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="26.71484375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="29.69921875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="247.40625" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="37.70703125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="107.01953125" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="42.34375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Add FSH code files and generated artifacts for May Connectathon
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bfs.xlsx
+++ b/build/output/StructureDefinition-pacio-bfs.xlsx
@@ -1455,47 +1455,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.6015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="44.67578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="66.26953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="67.91015625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="60.515625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="56.66015625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="63.703125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="57.1328125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="41.01953125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="26.71484375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="29.69921875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="247.40625" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="37.70703125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="107.01953125" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="42.34375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Add SelfCare, IADL, Device, UseOfDevice instances in FSH code
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bfs.xlsx
+++ b/build/output/StructureDefinition-pacio-bfs.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$53</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="426">
   <si>
     <t>Path</t>
   </si>
@@ -381,6 +381,19 @@
     <t>.participation[typeCode=LOC].role</t>
   </si>
   <si>
+    <t>device-use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://pacioproject.org/StructureDefinition/device-patient-used}
+</t>
+  </si>
+  <si>
+    <t>Optional Extensions Element</t>
+  </si>
+  <si>
+    <t>Optional Extension Element - found in all resources.</t>
+  </si>
+  <si>
     <t>Observation.modifierExtension</t>
   </si>
   <si>
@@ -748,7 +761,7 @@
     <t>Observation.performer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner)
+    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Organization|CareTeam|Patient|RelatedPerson)
 </t>
   </si>
   <si>
@@ -1488,7 +1501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO52"/>
+  <dimension ref="A1:AO53"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2714,13 +2727,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>116</v>
       </c>
-      <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2730,16 +2745,16 @@
         <v>44</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>45</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="K11" t="s" s="2">
         <v>118</v>
@@ -2747,12 +2762,8 @@
       <c r="L11" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="M11" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="N11" t="s" s="2">
-        <v>121</v>
-      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
         <v>45</v>
       </c>
@@ -2800,7 +2811,7 @@
         <v>45</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>43</v>
@@ -2809,7 +2820,7 @@
         <v>44</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="AI11" t="s" s="2">
         <v>106</v>
@@ -2835,11 +2846,11 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -2852,23 +2863,25 @@
         <v>45</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J12" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K12" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="L12" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="M12" t="s" s="2">
         <v>124</v>
       </c>
-      <c r="K12" t="s" s="2">
+      <c r="N12" t="s" s="2">
         <v>125</v>
-      </c>
-      <c r="L12" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" t="s" s="2">
-        <v>127</v>
       </c>
       <c r="O12" t="s" s="2">
         <v>45</v>
@@ -2917,7 +2930,7 @@
         <v>45</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>43</v>
@@ -2929,22 +2942,22 @@
         <v>45</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>129</v>
+        <v>45</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="AO12" t="s" s="2">
         <v>45</v>
@@ -2952,11 +2965,11 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
@@ -2975,17 +2988,17 @@
         <v>56</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" t="s" s="2">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="O13" t="s" s="2">
         <v>45</v>
@@ -3034,7 +3047,7 @@
         <v>45</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>43</v>
@@ -3049,19 +3062,19 @@
         <v>67</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="AO13" t="s" s="2">
         <v>45</v>
@@ -3069,11 +3082,11 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -3092,18 +3105,18 @@
         <v>56</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="N14" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" t="s" s="2">
+        <v>141</v>
+      </c>
       <c r="O14" t="s" s="2">
         <v>45</v>
       </c>
@@ -3151,7 +3164,7 @@
         <v>45</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>43</v>
@@ -3166,16 +3179,16 @@
         <v>67</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="AN14" t="s" s="2">
         <v>45</v>
@@ -3186,43 +3199,41 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I15" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>75</v>
+        <v>147</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>154</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>45</v>
       </c>
@@ -3246,13 +3257,13 @@
         <v>45</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>157</v>
+        <v>45</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3270,13 +3281,13 @@
         <v>45</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>45</v>
@@ -3285,19 +3296,19 @@
         <v>67</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>162</v>
+        <v>45</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3305,7 +3316,7 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3322,25 +3333,25 @@
         <v>45</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3365,13 +3376,13 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>79</v>
+        <v>159</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3389,13 +3400,13 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>45</v>
@@ -3404,19 +3415,19 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>45</v>
@@ -3424,11 +3435,11 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>174</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3444,22 +3455,22 @@
         <v>45</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3484,11 +3495,13 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="X17" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>173</v>
+      </c>
       <c r="Y17" t="s" s="2">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3506,13 +3519,13 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>45</v>
@@ -3521,31 +3534,31 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>185</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>45</v>
+        <v>178</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3564,19 +3577,19 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
@@ -3601,13 +3614,11 @@
         <v>45</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X18" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="X18" s="2"/>
       <c r="Y18" t="s" s="2">
-        <v>45</v>
+        <v>183</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>45</v>
@@ -3625,10 +3636,10 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>55</v>
@@ -3640,27 +3651,27 @@
         <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>45</v>
+        <v>185</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>45</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3668,10 +3679,10 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>45</v>
@@ -3683,18 +3694,20 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="N19" s="2"/>
+        <v>194</v>
+      </c>
+      <c r="N19" t="s" s="2">
+        <v>195</v>
+      </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
       </c>
@@ -3742,13 +3755,13 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>45</v>
@@ -3757,19 +3770,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>45</v>
+        <v>196</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3777,18 +3790,18 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>203</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>45</v>
@@ -3800,20 +3813,18 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="M20" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="K20" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>208</v>
-      </c>
+      <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>45</v>
       </c>
@@ -3861,13 +3872,13 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>45</v>
@@ -3876,19 +3887,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>209</v>
+        <v>45</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3896,11 +3907,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3919,19 +3930,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3980,7 +3991,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3995,19 +4006,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -4015,11 +4026,11 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>45</v>
+        <v>218</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -4038,18 +4049,20 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="N22" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>223</v>
+      </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
       </c>
@@ -4097,7 +4110,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4112,19 +4125,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>45</v>
+        <v>224</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4132,7 +4145,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4140,10 +4153,10 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s" s="2">
         <v>55</v>
-      </c>
-      <c r="F23" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>45</v>
@@ -4155,18 +4168,18 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="M23" s="2"/>
-      <c r="N23" t="s" s="2">
-        <v>236</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>45</v>
       </c>
@@ -4214,13 +4227,13 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>45</v>
@@ -4229,19 +4242,19 @@
         <v>67</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>237</v>
+        <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4249,7 +4262,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4257,10 +4270,10 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>45</v>
@@ -4272,19 +4285,17 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>164</v>
+        <v>237</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>244</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4333,42 +4344,42 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>246</v>
+        <v>45</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>45</v>
+        <v>241</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>45</v>
+        <v>244</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4388,22 +4399,22 @@
         <v>45</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4428,13 +4439,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>257</v>
+        <v>45</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4452,7 +4463,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4461,7 +4472,7 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4470,35 +4481,35 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>45</v>
+        <v>251</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>98</v>
+        <v>252</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>45</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>262</v>
+        <v>45</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>45</v>
@@ -4510,19 +4521,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4547,13 +4558,13 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4571,16 +4582,16 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>45</v>
+        <v>263</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>67</v>
@@ -4589,28 +4600,28 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>269</v>
+        <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>270</v>
+        <v>98</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>272</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>45</v>
+        <v>266</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
@@ -4629,19 +4640,19 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>274</v>
+        <v>168</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -4666,13 +4677,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>45</v>
+        <v>260</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>45</v>
+        <v>271</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>45</v>
+        <v>272</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4690,7 +4701,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4708,24 +4719,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>45</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4736,7 +4747,7 @@
         <v>43</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>45</v>
@@ -4748,18 +4759,20 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>164</v>
+        <v>278</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="N28" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="L28" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4783,13 +4796,13 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>285</v>
+        <v>45</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>286</v>
+        <v>45</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>287</v>
+        <v>45</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
@@ -4807,13 +4820,13 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>45</v>
@@ -4825,24 +4838,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>288</v>
+        <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>291</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4865,20 +4878,18 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>296</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4902,31 +4913,31 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="X29" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="Y29" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE29" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="X29" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="Y29" t="s" s="2">
-        <v>298</v>
-      </c>
-      <c r="Z29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE29" t="s" s="2">
-        <v>292</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4944,24 +4955,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>45</v>
+        <v>292</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>45</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4984,18 +4995,20 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>302</v>
+        <v>168</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="N30" s="2"/>
+        <v>299</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>300</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
       </c>
@@ -5019,13 +5032,13 @@
         <v>45</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>45</v>
+        <v>289</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>45</v>
+        <v>301</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>45</v>
+        <v>302</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>45</v>
@@ -5043,7 +5056,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5061,24 +5074,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>306</v>
+        <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>309</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5101,16 +5114,16 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5160,7 +5173,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5178,24 +5191,24 @@
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5206,7 +5219,7 @@
         <v>43</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>45</v>
@@ -5218,20 +5231,18 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>324</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>45</v>
       </c>
@@ -5279,42 +5290,42 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="AF32" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG32" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI32" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK32" t="s" s="2">
         <v>319</v>
       </c>
-      <c r="AF32" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG32" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI32" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK32" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="AL32" t="s" s="2">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>45</v>
+        <v>322</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5325,7 +5336,7 @@
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
@@ -5337,16 +5348,20 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>57</v>
+        <v>324</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+        <v>326</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="N33" t="s" s="2">
+        <v>328</v>
+      </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
       </c>
@@ -5394,31 +5409,31 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="AF33" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG33" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI33" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="AJ33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL33" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AM33" t="s" s="2">
         <v>331</v>
-      </c>
-      <c r="AF33" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG33" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="AH33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AM33" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5429,18 +5444,18 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>45</v>
@@ -5452,17 +5467,15 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>334</v>
       </c>
-      <c r="L34" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>120</v>
-      </c>
+      <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>45</v>
@@ -5511,31 +5524,31 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AF34" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG34" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM34" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="AF34" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG34" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI34" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5550,7 +5563,7 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>338</v>
+        <v>121</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -5563,26 +5576,24 @@
         <v>45</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
         <v>100</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="L35" t="s" s="2">
-        <v>340</v>
-      </c>
       <c r="M35" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>121</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5630,7 +5641,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5654,7 +5665,7 @@
         <v>45</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>98</v>
+        <v>336</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5665,39 +5676,43 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>45</v>
+        <v>342</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H36" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J36" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K36" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="K36" t="s" s="2">
+      <c r="L36" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="L36" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="M36" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>125</v>
+      </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
       </c>
@@ -5745,19 +5760,19 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>346</v>
+        <v>45</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>45</v>
@@ -5766,10 +5781,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>347</v>
+        <v>45</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>348</v>
+        <v>98</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5780,7 +5795,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5803,13 +5818,13 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5860,7 +5875,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5869,7 +5884,7 @@
         <v>55</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>67</v>
@@ -5881,7 +5896,7 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>352</v>
@@ -5918,7 +5933,7 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>164</v>
+        <v>347</v>
       </c>
       <c r="K38" t="s" s="2">
         <v>354</v>
@@ -5926,12 +5941,8 @@
       <c r="L38" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="M38" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>357</v>
-      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5955,13 +5966,13 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>358</v>
+        <v>45</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -5988,7 +5999,7 @@
         <v>55</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>45</v>
+        <v>350</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>67</v>
@@ -5997,13 +6008,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>360</v>
+        <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>271</v>
+        <v>356</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6014,7 +6025,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6025,7 +6036,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -6037,19 +6048,19 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6074,13 +6085,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>285</v>
+        <v>79</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6098,13 +6109,13 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>45</v>
@@ -6116,13 +6127,13 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6133,7 +6144,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6144,7 +6155,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>45</v>
@@ -6156,17 +6167,19 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="N40" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="K40" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6191,13 +6204,13 @@
         <v>45</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>45</v>
+        <v>289</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>45</v>
+        <v>371</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>45</v>
+        <v>372</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>45</v>
@@ -6215,13 +6228,13 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>45</v>
@@ -6233,13 +6246,13 @@
         <v>45</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>45</v>
+        <v>364</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>45</v>
+        <v>365</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>374</v>
+        <v>275</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6250,7 +6263,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6273,16 +6286,18 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>57</v>
+        <v>374</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" s="2"/>
+      <c r="N41" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
       </c>
@@ -6330,7 +6345,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6351,7 +6366,7 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>347</v>
+        <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>378</v>
@@ -6376,7 +6391,7 @@
         <v>43</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>45</v>
@@ -6385,20 +6400,18 @@
         <v>45</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="L42" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>383</v>
-      </c>
+      <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>45</v>
@@ -6453,7 +6466,7 @@
         <v>43</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>45</v>
@@ -6468,10 +6481,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>384</v>
+        <v>351</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6482,7 +6495,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6505,16 +6518,16 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="K43" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6564,7 +6577,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6585,10 +6598,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6599,7 +6612,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6622,20 +6635,18 @@
         <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>320</v>
+        <v>391</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>393</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="M44" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>396</v>
-      </c>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6683,7 +6694,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6704,10 +6715,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6718,7 +6729,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6729,7 +6740,7 @@
         <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6738,19 +6749,23 @@
         <v>45</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>57</v>
+        <v>324</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>329</v>
+        <v>397</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>398</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>400</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
@@ -6798,19 +6813,19 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>331</v>
+        <v>396</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>45</v>
@@ -6819,10 +6834,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>45</v>
+        <v>401</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>332</v>
+        <v>402</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6833,18 +6848,18 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>45</v>
@@ -6856,17 +6871,15 @@
         <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>334</v>
       </c>
-      <c r="L46" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>120</v>
-      </c>
+      <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>45</v>
@@ -6915,31 +6928,31 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AF46" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG46" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM46" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="AF46" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH46" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI46" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="AJ46" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK46" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL46" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AM46" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6950,11 +6963,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>338</v>
+        <v>121</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6967,26 +6980,24 @@
         <v>45</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
         <v>100</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="L47" t="s" s="2">
-        <v>340</v>
-      </c>
       <c r="M47" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>121</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>45</v>
       </c>
@@ -7034,7 +7045,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7058,7 +7069,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>98</v>
+        <v>336</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7069,42 +7080,42 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>45</v>
+        <v>342</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I48" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>403</v>
+        <v>343</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>404</v>
+        <v>344</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>405</v>
+        <v>124</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7129,13 +7140,13 @@
         <v>45</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>285</v>
+        <v>45</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>406</v>
+        <v>45</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>407</v>
+        <v>45</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>45</v>
@@ -7153,34 +7164,34 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>402</v>
+        <v>345</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>408</v>
+        <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>183</v>
+        <v>98</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>184</v>
+        <v>45</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>45</v>
@@ -7188,7 +7199,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7196,7 +7207,7 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F49" t="s" s="2">
         <v>55</v>
@@ -7211,19 +7222,19 @@
         <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>410</v>
+        <v>168</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>243</v>
+        <v>408</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>245</v>
+        <v>182</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7248,13 +7259,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>45</v>
+        <v>289</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>45</v>
+        <v>410</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>45</v>
+        <v>411</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7272,10 +7283,10 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>55</v>
@@ -7290,24 +7301,24 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>248</v>
+        <v>186</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>249</v>
+        <v>187</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>45</v>
+        <v>188</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7327,22 +7338,22 @@
         <v>45</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>164</v>
+        <v>414</v>
       </c>
       <c r="K50" t="s" s="2">
         <v>415</v>
       </c>
       <c r="L50" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="M50" t="s" s="2">
-        <v>417</v>
-      </c>
       <c r="N50" t="s" s="2">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7367,13 +7378,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>257</v>
+        <v>45</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7391,7 +7402,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7400,7 +7411,7 @@
         <v>55</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>259</v>
+        <v>45</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>67</v>
@@ -7409,19 +7420,19 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>45</v>
+        <v>417</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>98</v>
+        <v>252</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>45</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" hidden="true">
@@ -7430,14 +7441,14 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>262</v>
+        <v>45</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>45</v>
@@ -7449,19 +7460,19 @@
         <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>263</v>
+        <v>419</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>264</v>
+        <v>420</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>265</v>
+        <v>421</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7486,13 +7497,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7516,10 +7527,10 @@
         <v>43</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>45</v>
+        <v>263</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>67</v>
@@ -7528,28 +7539,28 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>269</v>
+        <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>270</v>
+        <v>98</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>272</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>45</v>
+        <v>266</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7568,19 +7579,19 @@
         <v>45</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>45</v>
+        <v>168</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>420</v>
+        <v>267</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>421</v>
+        <v>268</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>323</v>
+        <v>269</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>324</v>
+        <v>270</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7605,13 +7616,13 @@
         <v>45</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>45</v>
+        <v>260</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>45</v>
+        <v>271</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>45</v>
+        <v>272</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7629,7 +7640,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7647,23 +7658,142 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>326</v>
+        <v>274</v>
       </c>
       <c r="AM52" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO52" t="s" s="2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="M53" t="s" s="2">
         <v>327</v>
       </c>
-      <c r="AN52" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO52" t="s" s="2">
+      <c r="N53" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="O53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO53" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO52">
+  <autoFilter ref="A1:AO53">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7673,7 +7803,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI51">
+  <conditionalFormatting sqref="A2:AI52">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>